<commit_message>
adj: update contact count variable to use selected contacts
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\WhatsApp Service Joomla Plugin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EEA0C0-5DD3-420E-8AA8-03C5EFF65978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F352ECA-6872-4A7B-8CD6-C8235980554F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="1800" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Phone Numbers</t>
   </si>
@@ -39,12 +39,18 @@
   <si>
     <t>Testing dddd</t>
   </si>
+  <si>
+    <t>+6598940556</t>
+  </si>
+  <si>
+    <t>Tze ying SG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -54,6 +60,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -304,7 +315,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -337,7 +348,12 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3328,6 +3344,7 @@
       <c r="A1000" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>